<commit_message>
Regular Update on what's done
</commit_message>
<xml_diff>
--- a/Matlab files/Резултати.xlsx
+++ b/Matlab files/Резултати.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lyubo\Desktop\Master final thesis\Masters-Final-Thesis\Matlab files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C7E481-D448-4F23-BA1D-A921D3169538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD1720A-DA80-402D-8C9B-F8A64FBE2FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="70">
   <si>
     <t>Quadratic DA</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Gabor PCA + Shapes</t>
   </si>
   <si>
-    <t>Binarized image shapes</t>
-  </si>
-  <si>
     <t>1F+2F+3F+4F+5F</t>
   </si>
   <si>
@@ -169,12 +166,93 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,8,</t>
+  </si>
+  <si>
+    <t>Gabor PCA</t>
+  </si>
+  <si>
+    <t>3rd PC</t>
+  </si>
+  <si>
+    <t>4th PC</t>
+  </si>
+  <si>
+    <t>5th PC</t>
+  </si>
+  <si>
+    <t>6th PC</t>
+  </si>
+  <si>
+    <t>7th PC</t>
+  </si>
+  <si>
+    <t>8th PC</t>
+  </si>
+  <si>
+    <t>9th PC</t>
+  </si>
+  <si>
+    <t>10th PC</t>
+  </si>
+  <si>
+    <t>13th PC</t>
+  </si>
+  <si>
+    <t>15th PC</t>
+  </si>
+  <si>
+    <t>17th PC</t>
+  </si>
+  <si>
+    <t>19th PC</t>
+  </si>
+  <si>
+    <t>21st PC</t>
+  </si>
+  <si>
+    <t>11th PC</t>
+  </si>
+  <si>
+    <t>23rd PC</t>
+  </si>
+  <si>
+    <t>27th PC</t>
+  </si>
+  <si>
+    <t>30th PC</t>
+  </si>
+  <si>
+    <t>Габор Главни компоненти</t>
+  </si>
+  <si>
+    <t>Квадратичен ДА</t>
+  </si>
+  <si>
+    <t>Линеен ДА</t>
+  </si>
+  <si>
+    <t>МСПС (матрица за съвместна поява на сивото)Главни компоненти</t>
+  </si>
+  <si>
+    <t>4 свойства</t>
+  </si>
+  <si>
+    <t>МСПС (матрица за съвместна поява на сивото) 4 свойства</t>
+  </si>
+  <si>
+    <t>Локални бинарни модели Главни компоненти</t>
+  </si>
+  <si>
+    <t>Геометрична форма и размери - признаци</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,7 +296,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -226,11 +304,304 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -244,10 +615,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:O65"/>
+  <dimension ref="B2:Y65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -545,23 +986,28 @@
     <col min="13" max="13" width="27.90625" customWidth="1"/>
     <col min="14" max="14" width="12.26953125" customWidth="1"/>
     <col min="15" max="15" width="11.1796875" customWidth="1"/>
+    <col min="18" max="18" width="24.6328125" customWidth="1"/>
+    <col min="19" max="19" width="12.6328125" customWidth="1"/>
+    <col min="20" max="20" width="24.6328125" customWidth="1"/>
+    <col min="21" max="21" width="12.6328125" customWidth="1"/>
+    <col min="24" max="24" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="D2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="I2" s="47"/>
+      <c r="N2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="O2" s="47"/>
+    </row>
+    <row r="4" spans="3:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N4">
         <v>84</v>
       </c>
@@ -569,14 +1015,14 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="3:15" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
+    <row r="5" spans="3:23" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -597,15 +1043,27 @@
       <c r="O5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
+      <c r="R5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="11">
         <v>88.571399999999997</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="32">
         <v>87.428600000000003</v>
       </c>
       <c r="G6" t="s">
@@ -623,15 +1081,27 @@
       <c r="O6" s="2">
         <v>95.428600000000003</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+      <c r="R6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="17">
+        <v>59.428600000000003</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="22">
+        <v>56.571399999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="3:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="11">
         <v>94.285700000000006</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="33">
         <v>88.571399999999997</v>
       </c>
       <c r="G7" t="s">
@@ -643,15 +1113,27 @@
       <c r="I7" s="5">
         <v>90.285700000000006</v>
       </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+      <c r="R7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="15">
+        <v>67.428600000000003</v>
+      </c>
+      <c r="T7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="24">
+        <v>53.714300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="3:23" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="11">
         <v>94.285700000000006</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="33">
         <v>90.285700000000006</v>
       </c>
       <c r="G8" t="s">
@@ -663,24 +1145,36 @@
       <c r="I8" s="5">
         <v>90.285700000000006</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="N8" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="46" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="R8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="15">
+        <v>66.285700000000006</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U8" s="24">
+        <v>61.714300000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="11">
         <v>95.428600000000003</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="33">
         <v>90.285700000000006</v>
       </c>
       <c r="G9" t="s">
@@ -692,24 +1186,36 @@
       <c r="I9" s="5">
         <v>93.714299999999994</v>
       </c>
-      <c r="M9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9">
+      <c r="M9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="16">
         <v>73.142899999999997</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="44">
         <v>74.285700000000006</v>
       </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+      <c r="R9" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="S9" s="15">
+        <v>74.285700000000006</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="24">
+        <v>69.714299999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="11">
         <v>94.857100000000003</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="33">
         <v>91.428600000000003</v>
       </c>
       <c r="G10" t="s">
@@ -721,24 +1227,36 @@
       <c r="I10" s="5">
         <v>93.714299999999994</v>
       </c>
-      <c r="M10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10">
+      <c r="M10" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="14">
         <v>69.714299999999994</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="37">
         <v>74.857100000000003</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+      <c r="R10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" s="15">
+        <v>77.714299999999994</v>
+      </c>
+      <c r="T10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="24">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="34">
         <v>98.285700000000006</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="33">
         <v>92</v>
       </c>
       <c r="G11" t="s">
@@ -750,24 +1268,36 @@
       <c r="I11" s="5">
         <v>95.428600000000003</v>
       </c>
-      <c r="M11" t="s">
-        <v>31</v>
-      </c>
-      <c r="N11">
+      <c r="M11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" s="14">
         <v>72</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="37">
         <v>68.571399999999997</v>
       </c>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
+      <c r="R11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="S11" s="15">
+        <v>80.571399999999997</v>
+      </c>
+      <c r="T11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" s="24">
+        <v>71.428600000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="11">
         <v>97.142899999999997</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="33">
         <v>91.428600000000003</v>
       </c>
       <c r="G12" t="s">
@@ -779,24 +1309,36 @@
       <c r="I12" s="2">
         <v>96</v>
       </c>
-      <c r="M12" t="s">
-        <v>32</v>
-      </c>
-      <c r="N12">
+      <c r="M12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12" s="14">
         <v>73.142899999999997</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="37">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+      <c r="R12" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="S12" s="15">
+        <v>80</v>
+      </c>
+      <c r="T12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="U12" s="24">
+        <v>71.428600000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="11">
         <v>96.571399999999997</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="33">
         <v>90.857100000000003</v>
       </c>
       <c r="G13" t="s">
@@ -808,24 +1350,36 @@
       <c r="I13" s="5">
         <v>95.428600000000003</v>
       </c>
-      <c r="M13" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13">
+      <c r="M13" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="14">
         <v>73.714299999999994</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="37">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
+      <c r="R13" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="15">
+        <v>79.428600000000003</v>
+      </c>
+      <c r="T13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="24">
+        <v>74.857100000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="11">
         <v>94.857100000000003</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="33">
         <v>90.285700000000006</v>
       </c>
       <c r="G14" t="s">
@@ -837,24 +1391,36 @@
       <c r="I14" s="5">
         <v>95.428600000000003</v>
       </c>
-      <c r="M14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N14">
+      <c r="M14" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="N14" s="14">
         <v>71.428600000000003</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="41">
         <v>76.571399999999997</v>
       </c>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
+      <c r="R14" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="S14" s="15">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="T14" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="U14" s="24">
+        <v>83.428600000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="3:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="11">
         <v>93.714299999999994</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="33">
         <v>92.571399999999997</v>
       </c>
       <c r="G15" t="s">
@@ -866,24 +1432,40 @@
       <c r="I15" s="5">
         <v>95.428600000000003</v>
       </c>
-      <c r="M15" t="s">
-        <v>33</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="M15" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="43">
         <v>76.571399999999997</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="42">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C16" t="s">
+      <c r="R15" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="S15" s="28">
+        <v>88.571399999999997</v>
+      </c>
+      <c r="T15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="U15" s="29">
+        <v>84.571399999999997</v>
+      </c>
+      <c r="W15">
+        <f>100-U15</f>
+        <v>15.428600000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="3:23" x14ac:dyDescent="0.35">
+      <c r="C16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="11">
         <v>92.571399999999997</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="33">
         <v>92.571399999999997</v>
       </c>
       <c r="G16" t="s">
@@ -895,15 +1477,19 @@
       <c r="I16" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
+      <c r="R16" s="11"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="27"/>
+    </row>
+    <row r="17" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="11">
         <v>92</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="33">
         <v>93.714299999999994</v>
       </c>
       <c r="G17" t="s">
@@ -915,15 +1501,19 @@
       <c r="I17" s="2">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
+      <c r="R17" s="11"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="27"/>
+    </row>
+    <row r="18" spans="2:23" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="13">
         <v>92.571399999999997</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="35">
         <v>94.285700000000006</v>
       </c>
       <c r="G18" t="s">
@@ -935,17 +1525,24 @@
       <c r="I18" s="5">
         <v>95.428600000000003</v>
       </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19">
-        <v>90.857100000000003</v>
-      </c>
-      <c r="E19" s="2">
-        <v>94.285700000000006</v>
-      </c>
+      <c r="R18" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="S18" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T18" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="U18" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="G19" t="s">
         <v>18</v>
       </c>
@@ -955,17 +1552,25 @@
       <c r="I19" s="5">
         <v>95.428600000000003</v>
       </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20">
+      <c r="R19" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" s="16">
+        <v>88.571399999999997</v>
+      </c>
+      <c r="T19" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U19" s="22">
         <v>87.428600000000003</v>
       </c>
-      <c r="E20">
-        <v>93.142899999999997</v>
-      </c>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="G20" t="s">
         <v>16</v>
       </c>
@@ -975,17 +1580,28 @@
       <c r="I20" s="5">
         <v>94.857100000000003</v>
       </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <v>82.857100000000003</v>
-      </c>
-      <c r="E21">
-        <v>93.142899999999997</v>
-      </c>
+      <c r="R20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S20" s="14">
+        <v>94.285700000000006</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U20" s="37">
+        <v>88.571399999999997</v>
+      </c>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
+        <f>100-E18</f>
+        <v>5.7142999999999944</v>
+      </c>
+      <c r="E21" s="5"/>
       <c r="G21" t="s">
         <v>19</v>
       </c>
@@ -995,17 +1611,28 @@
       <c r="I21" s="5">
         <v>94.285700000000006</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22">
-        <v>80.571399999999997</v>
-      </c>
-      <c r="E22">
-        <v>92.571399999999997</v>
-      </c>
+      <c r="R21" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" s="14">
+        <v>94.285700000000006</v>
+      </c>
+      <c r="T21" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U21" s="37">
+        <v>90.285700000000006</v>
+      </c>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5">
+        <f>100-D11</f>
+        <v>1.7142999999999944</v>
+      </c>
+      <c r="E22" s="5"/>
       <c r="G22" t="s">
         <v>20</v>
       </c>
@@ -1015,17 +1642,25 @@
       <c r="I22" s="5">
         <v>94.285700000000006</v>
       </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="3">
-        <v>70.857100000000003</v>
-      </c>
-      <c r="E23">
-        <v>92.571399999999997</v>
-      </c>
+      <c r="R22" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="S22" s="14">
+        <v>95.428600000000003</v>
+      </c>
+      <c r="T22" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="U22" s="37">
+        <v>90.285700000000006</v>
+      </c>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="G23" t="s">
         <v>21</v>
       </c>
@@ -1033,183 +1668,630 @@
       <c r="I23" s="5">
         <v>94.285700000000006</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G26" s="4" t="s">
+      <c r="R23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="S23" s="14">
+        <v>94.857100000000003</v>
+      </c>
+      <c r="T23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U23" s="37">
+        <v>91.428600000000003</v>
+      </c>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="R24" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="S24" s="36">
+        <v>98.285700000000006</v>
+      </c>
+      <c r="T24" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="U24" s="37">
+        <v>92</v>
+      </c>
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R25" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="14">
+        <v>97.142899999999997</v>
+      </c>
+      <c r="T25" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="U25" s="37">
+        <v>91.428600000000003</v>
+      </c>
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G26" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="I26" s="54" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G27" t="s">
+      <c r="R26" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="S26" s="14">
+        <v>96.571399999999997</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="U26" s="37">
+        <v>90.857100000000003</v>
+      </c>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="G27" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5">
+      <c r="H27" s="52"/>
+      <c r="I27" s="22">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G28" t="s">
+      <c r="R27" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="S27" s="14">
+        <v>94.857100000000003</v>
+      </c>
+      <c r="T27" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U27" s="37">
+        <v>90.285700000000006</v>
+      </c>
+      <c r="W27" s="11"/>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="G28" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5">
+      <c r="H28" s="48"/>
+      <c r="I28" s="24">
         <v>86.857100000000003</v>
       </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G29" t="s">
+      <c r="R28" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="S28" s="14">
+        <v>93.714299999999994</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="U28" s="37">
+        <v>92.571399999999997</v>
+      </c>
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="C29" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5">
+      <c r="H29" s="48"/>
+      <c r="I29" s="24">
         <v>87.428600000000003</v>
       </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G30" t="s">
+      <c r="R29" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="S29" s="14">
+        <v>92.571399999999997</v>
+      </c>
+      <c r="T29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="U29" s="37">
+        <v>92.571399999999997</v>
+      </c>
+      <c r="W29" s="11"/>
+    </row>
+    <row r="30" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="5">
+        <v>59.428600000000003</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="G30" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5">
+      <c r="H30" s="48"/>
+      <c r="I30" s="24">
         <v>88.571399999999997</v>
       </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G31" t="s">
+      <c r="R30" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="S30" s="14">
+        <v>92</v>
+      </c>
+      <c r="T30" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="U30" s="37">
+        <v>93.714299999999994</v>
+      </c>
+      <c r="W30" s="11"/>
+    </row>
+    <row r="31" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="5">
+        <v>67.428600000000003</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="G31" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5">
+      <c r="H31" s="48"/>
+      <c r="I31" s="24">
         <v>88.571399999999997</v>
       </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G32" t="s">
+      <c r="R31" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="S31" s="26">
+        <v>92.571399999999997</v>
+      </c>
+      <c r="T31" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="U31" s="29">
+        <v>94.285700000000006</v>
+      </c>
+      <c r="W31" s="11"/>
+    </row>
+    <row r="32" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="5">
+        <v>66.285700000000006</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="G32" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5">
+      <c r="H32" s="48"/>
+      <c r="I32" s="24">
         <v>89.142899999999997</v>
       </c>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G33" t="s">
+    <row r="33" spans="3:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="5">
+        <v>74.285700000000006</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="G33" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5">
+      <c r="H33" s="48"/>
+      <c r="I33" s="24">
         <v>88.571399999999997</v>
       </c>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G34" t="s">
+    <row r="34" spans="3:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="5">
+        <v>77.714299999999994</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="G34" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5">
+      <c r="H34" s="48"/>
+      <c r="I34" s="24">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G35" t="s">
+      <c r="R34" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="S34" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T34" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="U34" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="X34" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y34" s="54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="5">
+        <v>80.571399999999997</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="G35" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5">
+      <c r="H35" s="48"/>
+      <c r="I35" s="24">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G36" t="s">
+      <c r="R35" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="S35" s="40">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="T35" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="U35" s="40">
+        <v>86.857100000000003</v>
+      </c>
+      <c r="X35" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y35" s="22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36" s="5">
+        <v>80</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="G36" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5">
+      <c r="H36" s="48"/>
+      <c r="I36" s="24">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G37" t="s">
+      <c r="X36" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y36" s="24">
+        <v>86.857100000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="3:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="5">
+        <v>79.428600000000003</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="G37" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5">
+      <c r="H37" s="48"/>
+      <c r="I37" s="24">
         <v>88.571399999999997</v>
       </c>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G38" t="s">
+      <c r="X37" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y37" s="24">
+        <v>87.428600000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="3:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="5">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="G38" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5">
+      <c r="H38" s="48"/>
+      <c r="I38" s="24">
         <v>89.714299999999994</v>
       </c>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G39" t="s">
+      <c r="R38" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="S38" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T38" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="U38" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="X38" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y38" s="24">
+        <v>88.571399999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="2">
+        <v>88.571399999999997</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="G39" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5">
+      <c r="H39" s="48"/>
+      <c r="I39" s="24">
         <v>89.714299999999994</v>
       </c>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G40" t="s">
+      <c r="R39" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S39" s="16">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="T39" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U39" s="22">
+        <v>79.428600000000003</v>
+      </c>
+      <c r="X39" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y39" s="24">
+        <v>88.571399999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="5">
+        <v>86.285700000000006</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="G40" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="6"/>
-      <c r="I40" s="5">
+      <c r="H40" s="49"/>
+      <c r="I40" s="24">
         <v>88</v>
       </c>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G41" t="s">
+      <c r="R40" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S40" s="14">
+        <v>82.285700000000006</v>
+      </c>
+      <c r="T40" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="U40" s="37">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="X40" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y40" s="24">
+        <v>89.142899999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41" s="5">
+        <v>84.571399999999997</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="G41" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="6"/>
-      <c r="I41" s="5">
+      <c r="H41" s="49"/>
+      <c r="I41" s="24">
         <v>89.714299999999994</v>
       </c>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G42" t="s">
+      <c r="R41" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="S41" s="14">
+        <v>78.857100000000003</v>
+      </c>
+      <c r="T41" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="U41" s="37">
+        <v>82.285700000000006</v>
+      </c>
+      <c r="X41" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y41" s="24">
+        <v>88.571399999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="G42" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H42" s="6"/>
-      <c r="I42" s="5">
+      <c r="H42" s="49"/>
+      <c r="I42" s="24">
         <v>89.714299999999994</v>
       </c>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G43" t="s">
+      <c r="R42" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="S42" s="14">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="T42" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="U42" s="37">
+        <v>78.857100000000003</v>
+      </c>
+      <c r="X42" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y42" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="G43" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H43" s="6"/>
-      <c r="I43" s="2">
+      <c r="H43" s="49"/>
+      <c r="I43" s="41">
         <v>90.285700000000006</v>
       </c>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G44" t="s">
+      <c r="R43" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="S43" s="14">
+        <v>83.428600000000003</v>
+      </c>
+      <c r="T43" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="U43" s="37">
+        <v>80.571399999999997</v>
+      </c>
+      <c r="X43" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y43" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="G44" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5">
+      <c r="H44" s="50"/>
+      <c r="I44" s="51">
         <v>89.714299999999994</v>
       </c>
-    </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="R44" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="S44" s="14">
+        <v>85.142899999999997</v>
+      </c>
+      <c r="T44" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="U44" s="37">
+        <v>81.714299999999994</v>
+      </c>
+      <c r="X44" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y44" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="R45" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="S45" s="14">
+        <v>85.142899999999997</v>
+      </c>
+      <c r="T45" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="U45" s="37">
+        <v>83.428600000000003</v>
+      </c>
+      <c r="X45" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y45" s="24">
+        <v>88.571399999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="R46" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="S46" s="14">
+        <v>85.714299999999994</v>
+      </c>
+      <c r="T46" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="U46" s="37">
+        <v>83.428600000000003</v>
+      </c>
+      <c r="X46" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y46" s="24">
+        <v>89.714299999999994</v>
+      </c>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.35">
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
       <c r="G47" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>0</v>
@@ -1217,10 +2299,28 @@
       <c r="I47" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="R47" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="S47" s="36">
+        <v>87.428600000000003</v>
+      </c>
+      <c r="T47" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U47" s="37">
+        <v>87.428600000000003</v>
+      </c>
+      <c r="X47" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y47" s="24">
+        <v>89.714299999999994</v>
+      </c>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.35">
       <c r="G48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H48" s="5">
         <v>88.571399999999997</v>
@@ -1228,10 +2328,28 @@
       <c r="I48" s="5">
         <v>93.714299999999994</v>
       </c>
-    </row>
-    <row r="49" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="R48" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="S48" s="14">
+        <v>86.857100000000003</v>
+      </c>
+      <c r="T48" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="U48" s="37">
+        <v>87.428600000000003</v>
+      </c>
+      <c r="X48" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y48" s="24">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H49" s="5">
         <v>90.285700000000006</v>
@@ -1239,10 +2357,28 @@
       <c r="I49" s="5">
         <v>93.142899999999997</v>
       </c>
-    </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="R49" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="S49" s="14">
+        <v>83.428600000000003</v>
+      </c>
+      <c r="T49" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="U49" s="37">
+        <v>87.428600000000003</v>
+      </c>
+      <c r="X49" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y49" s="24">
+        <v>89.714299999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H50" s="5">
         <v>89.714299999999994</v>
@@ -1251,10 +2387,28 @@
         <v>93.714299999999994</v>
       </c>
       <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="R50" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="S50" s="14">
+        <v>83.428600000000003</v>
+      </c>
+      <c r="T50" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="U50" s="37">
+        <v>89.142899999999997</v>
+      </c>
+      <c r="X50" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y50" s="24">
+        <v>89.714299999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H51" s="5">
         <v>89.142899999999997</v>
@@ -1262,10 +2416,28 @@
       <c r="I51" s="5">
         <v>93.714299999999994</v>
       </c>
-    </row>
-    <row r="52" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="R51" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="S51" s="14">
+        <v>82.857100000000003</v>
+      </c>
+      <c r="T51" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="U51" s="37">
+        <v>89.142899999999997</v>
+      </c>
+      <c r="X51" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y51" s="41">
+        <v>90.285700000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="7:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H52" s="5">
         <v>90.285700000000006</v>
@@ -1273,10 +2445,28 @@
       <c r="I52" s="5">
         <v>93.142899999999997</v>
       </c>
-    </row>
-    <row r="53" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="R52" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="S52" s="26">
+        <v>84.571399999999997</v>
+      </c>
+      <c r="T52" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="U52" s="29">
+        <v>90.285700000000006</v>
+      </c>
+      <c r="X52" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y52" s="51">
+        <v>89.714299999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H53" s="5">
         <v>90.857100000000003</v>
@@ -1285,9 +2475,9 @@
         <v>93.142899999999997</v>
       </c>
     </row>
-    <row r="54" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H54" s="5">
         <v>91.428600000000003</v>
@@ -1296,9 +2486,9 @@
         <v>94.285700000000006</v>
       </c>
     </row>
-    <row r="55" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H55" s="5">
         <v>90.285700000000006</v>
@@ -1306,11 +2496,11 @@
       <c r="I55" s="5">
         <v>94.285700000000006</v>
       </c>
-      <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="J55" s="7"/>
+    </row>
+    <row r="56" spans="7:25" x14ac:dyDescent="0.35">
       <c r="G56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H56" s="2">
         <v>92</v>
@@ -1319,37 +2509,37 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H57" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H61" s="6"/>
       <c r="I61" s="5"/>
     </row>
-    <row r="62" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H62" s="6"/>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H63" s="6"/>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="7:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="7:25" x14ac:dyDescent="0.35">
       <c r="H64" s="6"/>
       <c r="I64" s="5"/>
     </row>

</xml_diff>